<commit_message>
further refactor of DCA analysis. test passing. ready for user testing
</commit_message>
<xml_diff>
--- a/tests/resources/dca_print.xlsx
+++ b/tests/resources/dca_print.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_19_20" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_18_19" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_19_20" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_18_19" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -347,24 +346,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="B3:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -914,7 +895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
dca analysis added to cli
</commit_message>
<xml_diff>
--- a/tests/resources/dca_print.xlsx
+++ b/tests/resources/dca_print.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_19_20" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_18_19" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_17_18" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -346,561 +345,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:E40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Departmental DCA</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Costs</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Proportion costs</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10273</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.01831566485881267</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Amber/Green</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>67326</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.1200350873439522</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Amber</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>498</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.0008878809597672254</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Amber/Red</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>482789</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.8607613668374678</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>6</v>
-      </c>
-      <c r="D10" t="n">
-        <v>560886</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>SRO Finance confidence</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Costs</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Proportion costs</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>2</v>
-      </c>
-      <c r="D14" t="n">
-        <v>10273</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.01831566485881267</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Amber/Green</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Amber</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>4</v>
-      </c>
-      <c r="D16" t="n">
-        <v>550613</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.9816843351411874</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Amber/Red</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>6</v>
-      </c>
-      <c r="D20" t="n">
-        <v>560886</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>SRO Benefits RAG</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Costs</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Proportion costs</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>2</v>
-      </c>
-      <c r="D24" t="n">
-        <v>4302</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.007670007809073501</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Amber/Green</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Amber</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>4</v>
-      </c>
-      <c r="D26" t="n">
-        <v>556584</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.9923299921909265</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Amber/Red</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>6</v>
-      </c>
-      <c r="D30" t="n">
-        <v>560886</v>
-      </c>
-      <c r="E30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>SRO Schedule Confidence</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Count</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Costs</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Proportion costs</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>2</v>
-      </c>
-      <c r="D34" t="n">
-        <v>10273</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.01831566485881267</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Amber/Green</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Amber</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>3</v>
-      </c>
-      <c r="D36" t="n">
-        <v>550515</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.9815096115788235</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Amber/Red</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Red</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" t="n">
-        <v>98</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.0001747235623638315</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>6</v>
-      </c>
-      <c r="D40" t="n">
-        <v>560886</v>
-      </c>
-      <c r="E40" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="B3:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -957,10 +401,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>1188</v>
+        <v>60</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1378030390905927</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6">
@@ -970,13 +414,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>7433</v>
+        <v>70</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8621969609094072</v>
+        <v>0.4666666666666667</v>
       </c>
     </row>
     <row r="7">
@@ -986,13 +430,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.1333333333333333</v>
       </c>
     </row>
     <row r="8">
@@ -1037,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>8621</v>
+        <v>150</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -1075,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>672</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07794919382902216</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="15">
@@ -1107,10 +551,10 @@
         <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>7949</v>
+        <v>140</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9220508061709779</v>
+        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="17">
@@ -1171,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>8621</v>
+        <v>150</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -1206,13 +650,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="25">
@@ -1241,10 +685,10 @@
         <v>4</v>
       </c>
       <c r="D26" t="n">
-        <v>8353</v>
+        <v>140</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9689131191277114</v>
+        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="27">
@@ -1286,13 +730,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>268</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0310868808722886</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1305,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="n">
-        <v>8621</v>
+        <v>150</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
more refactoring of milestone data and graph compilation. most tests passing but not yet all.
</commit_message>
<xml_diff>
--- a/tests/resources/dca_print.xlsx
+++ b/tests/resources/dca_print.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:E30"/>
+  <dimension ref="B3:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -755,6 +755,140 @@
         <v>1</v>
       </c>
     </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Overall Resource DCA - Now</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Proportion costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" t="n">
+        <v>130</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Amber/Green</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Amber</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>20</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.1333333333333333</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Amber/Red</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>5</v>
+      </c>
+      <c r="D40" t="n">
+        <v>150</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor dcas and summaries
</commit_message>
<xml_diff>
--- a/tests/resources/dca_print.xlsx
+++ b/tests/resources/dca_print.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_17_18" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_19_20" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_18_19" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -345,6 +346,695 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B3:E50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Departmental DCA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Proportion costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10273</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01831566485881267</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Amber/Green</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>67326</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1200350873439522</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Amber</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>498</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0008878809597672254</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Amber/Red</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>482789</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8607613668374678</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>560886</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SRO Finance confidence</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Proportion costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10273</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.01831566485881267</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Amber/Green</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Amber</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>550613</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.9816843351411874</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Amber/Red</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" t="n">
+        <v>560886</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SRO Benefits RAG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Proportion costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="n">
+        <v>4302</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.007670007809073501</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Amber/Green</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Amber</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" t="n">
+        <v>556584</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9923299921909265</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Amber/Red</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>6</v>
+      </c>
+      <c r="D30" t="n">
+        <v>560886</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SRO Schedule Confidence</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Proportion costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="n">
+        <v>10273</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.01831566485881267</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Amber/Green</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Amber</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>3</v>
+      </c>
+      <c r="D36" t="n">
+        <v>550515</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.9815096115788235</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Amber/Red</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>98</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.0001747235623638315</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>6</v>
+      </c>
+      <c r="D40" t="n">
+        <v>560886</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Overall Resource DCA - Now</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Proportion costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Amber/Green</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Amber</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Amber/Red</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>6</v>
+      </c>
+      <c r="D49" t="n">
+        <v>560886</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>6</v>
+      </c>
+      <c r="D50" t="n">
+        <v>560886</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="B3:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -401,10 +1091,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>60</v>
+        <v>1188</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4</v>
+        <v>0.1378030390905927</v>
       </c>
     </row>
     <row r="6">
@@ -414,13 +1104,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>70</v>
+        <v>7433</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.8621969609094072</v>
       </c>
     </row>
     <row r="7">
@@ -430,13 +1120,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -481,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>150</v>
+        <v>8621</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -519,10 +1209,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>672</v>
       </c>
       <c r="E14" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.07794919382902216</v>
       </c>
     </row>
     <row r="15">
@@ -551,10 +1241,10 @@
         <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>140</v>
+        <v>7949</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9220508061709779</v>
       </c>
     </row>
     <row r="17">
@@ -615,7 +1305,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>150</v>
+        <v>8621</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -650,13 +1340,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.06666666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -685,10 +1375,10 @@
         <v>4</v>
       </c>
       <c r="D26" t="n">
-        <v>140</v>
+        <v>8353</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9689131191277114</v>
       </c>
     </row>
     <row r="27">
@@ -730,13 +1420,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>268</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>0.0310868808722886</v>
       </c>
     </row>
     <row r="30">
@@ -749,7 +1439,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="n">
-        <v>150</v>
+        <v>8621</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -784,13 +1474,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>130</v>
+        <v>1188</v>
       </c>
       <c r="E34" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.1378030390905927</v>
       </c>
     </row>
     <row r="35">
@@ -816,13 +1506,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" t="n">
-        <v>20</v>
+        <v>7433</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.8621969609094072</v>
       </c>
     </row>
     <row r="37">
@@ -883,7 +1573,7 @@
         <v>5</v>
       </c>
       <c r="D40" t="n">
-        <v>150</v>
+        <v>8621</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
wp refactor of tests
</commit_message>
<xml_diff>
--- a/tests/resources/dca_print.xlsx
+++ b/tests/resources/dca_print.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_19_20" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_18_19" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q1_20_21" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_19_20" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -357,7 +357,7 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Departmental DCA</t>
+          <t>SRO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -383,13 +383,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>10273</v>
+        <v>469.7</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01831566485881267</v>
+        <v>0.02622854943985702</v>
       </c>
     </row>
     <row r="5">
@@ -399,13 +399,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>67326</v>
+        <v>10686.66708285521</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1200350873439522</v>
+        <v>0.5967548987225048</v>
       </c>
     </row>
     <row r="6">
@@ -415,13 +415,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>498</v>
+        <v>6751.6</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0008878809597672254</v>
+        <v>0.3770165518376383</v>
       </c>
     </row>
     <row r="7">
@@ -431,13 +431,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>482789</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8607613668374678</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -479,10 +479,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>560886</v>
+        <v>17907.96708285521</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -491,7 +491,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>SRO Finance confidence</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -517,13 +517,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>10273</v>
+        <v>469.7</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01831566485881267</v>
+        <v>0.02622854943985702</v>
       </c>
     </row>
     <row r="15">
@@ -533,13 +533,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>7964.63</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.4447534420378293</v>
       </c>
     </row>
     <row r="16">
@@ -549,13 +549,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
-        <v>550613</v>
+        <v>9473.63708285521</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9816843351411874</v>
+        <v>0.5290180085223137</v>
       </c>
     </row>
     <row r="17">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>560886</v>
+        <v>17907.96708285521</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -625,7 +625,7 @@
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>SRO Benefits RAG</t>
+          <t>Benefits</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -651,13 +651,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>4302</v>
+        <v>1478.68</v>
       </c>
       <c r="E24" t="n">
-        <v>0.007670007809073501</v>
+        <v>0.08257106980142173</v>
       </c>
     </row>
     <row r="25">
@@ -667,13 +667,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>9207.98708285521</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.5141838289210832</v>
       </c>
     </row>
     <row r="26">
@@ -683,13 +683,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>556584</v>
+        <v>7221.3</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9923299921909265</v>
+        <v>0.4032451012774953</v>
       </c>
     </row>
     <row r="27">
@@ -747,10 +747,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" t="n">
-        <v>560886</v>
+        <v>17907.96708285521</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -759,7 +759,7 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>SRO Schedule Confidence</t>
+          <t>Schedule</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -785,13 +785,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D34" t="n">
-        <v>10273</v>
+        <v>11156.36708285521</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01831566485881267</v>
+        <v>0.6229834481623618</v>
       </c>
     </row>
     <row r="35">
@@ -817,13 +817,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>550515</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0.9815096115788235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -833,13 +833,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>6751.6</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>0.3770165518376383</v>
       </c>
     </row>
     <row r="38">
@@ -849,13 +849,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0001747235623638315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -881,10 +881,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" t="n">
-        <v>560886</v>
+        <v>17907.96708285521</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
@@ -893,7 +893,7 @@
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>Overall Resource DCA - Now</t>
+          <t>Resource</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -919,13 +919,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>7221.3</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>0.4032451012774953</v>
       </c>
     </row>
     <row r="45">
@@ -935,13 +935,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>10686.66708285521</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>0.5967548987225048</v>
       </c>
     </row>
     <row r="46">
@@ -999,13 +999,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>560886</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1015,10 +1015,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50" t="n">
-        <v>560886</v>
+        <v>17907.96708285521</v>
       </c>
       <c r="E50" t="n">
         <v>1</v>
@@ -1035,7 +1035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:E40"/>
+  <dimension ref="B3:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1046,7 +1046,7 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Departmental DCA</t>
+          <t>SRO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1072,13 +1072,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2118.6</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.1202439341118181</v>
       </c>
     </row>
     <row r="5">
@@ -1088,13 +1088,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1188</v>
+        <v>6490.37</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1378030390905927</v>
+        <v>0.3683694999723029</v>
       </c>
     </row>
     <row r="6">
@@ -1104,13 +1104,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>7433</v>
+        <v>9010.214</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8621969609094072</v>
+        <v>0.5113865659158791</v>
       </c>
     </row>
     <row r="7">
@@ -1171,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="n">
-        <v>8621</v>
+        <v>17619.184</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -1180,7 +1180,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>SRO Finance confidence</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1206,13 +1206,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>672</v>
+        <v>2118.6</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07794919382902216</v>
+        <v>0.1202439341118181</v>
       </c>
     </row>
     <row r="15">
@@ -1238,13 +1238,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
-        <v>7949</v>
+        <v>15500.584</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9220508061709779</v>
+        <v>0.8797560658881819</v>
       </c>
     </row>
     <row r="17">
@@ -1305,7 +1305,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>8621</v>
+        <v>17619.184</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -1314,7 +1314,7 @@
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>SRO Benefits RAG</t>
+          <t>Benefits</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1340,13 +1340,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>4064.784</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.2307021709972494</v>
       </c>
     </row>
     <row r="25">
@@ -1372,13 +1372,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" t="n">
-        <v>8353</v>
+        <v>13554.4</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9689131191277114</v>
+        <v>0.7692978290027507</v>
       </c>
     </row>
     <row r="27">
@@ -1420,13 +1420,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>268</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0310868808722886</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1439,7 +1439,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="n">
-        <v>8621</v>
+        <v>17619.184</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -1448,7 +1448,7 @@
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>Overall Resource DCA - Now</t>
+          <t>Schedule</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1477,10 +1477,10 @@
         <v>2</v>
       </c>
       <c r="D34" t="n">
-        <v>1188</v>
+        <v>2118.6</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1378030390905927</v>
+        <v>0.1202439341118181</v>
       </c>
     </row>
     <row r="35">
@@ -1506,13 +1506,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" t="n">
-        <v>7433</v>
+        <v>9108.853999999999</v>
       </c>
       <c r="E36" t="n">
-        <v>0.8621969609094072</v>
+        <v>0.5169850090673893</v>
       </c>
     </row>
     <row r="37">
@@ -1538,13 +1538,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>6391.73</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>0.3627710568207926</v>
       </c>
     </row>
     <row r="39">
@@ -1573,9 +1573,143 @@
         <v>5</v>
       </c>
       <c r="D40" t="n">
-        <v>8621</v>
+        <v>17619.184</v>
       </c>
       <c r="E40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Resource</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Costs</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Proportion costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>5</v>
+      </c>
+      <c r="D44" t="n">
+        <v>17619.184</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Amber/Green</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Amber</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Amber/Red</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>5</v>
+      </c>
+      <c r="D50" t="n">
+        <v>17619.184</v>
+      </c>
+      <c r="E50" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>